<commit_message>
session added, get data from excel changed
</commit_message>
<xml_diff>
--- a/attributes_mto.xlsx
+++ b/attributes_mto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demidov_ai\Documents\Демидов\Питон\appius-neosintez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demid\Documents\INK\python_ink\appius-mto-neosintez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E18FC8-7DD6-4763-8C37-CCFC909FC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8F07C7-C2E7-48E9-8418-375FBF150929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Количество уведомление об отгрузке</t>
   </si>
   <si>
-    <t>bbb4bf34-cc70-e911-8115-817c3f53a992</t>
-  </si>
-  <si>
     <t>Количество приход</t>
   </si>
   <si>
@@ -342,12 +339,6 @@
     <t>c7ec82e0-f360-e911-8115-817c3f53a992</t>
   </si>
   <si>
-    <t>532d2888-3582-ec11-911c-005056b6948b</t>
-  </si>
-  <si>
-    <t>^(\S*)\s</t>
-  </si>
-  <si>
     <t>regexp</t>
   </si>
   <si>
@@ -357,19 +348,13 @@
     <t>№ поз. По ГП</t>
   </si>
   <si>
-    <t>Тип материала</t>
-  </si>
-  <si>
-    <t>52ad3a8a-3382-ec11-911c-005056b6948b</t>
-  </si>
-  <si>
-    <t>708c334d-e78a-ec11-911c-005056b6948b</t>
-  </si>
-  <si>
     <t>7e2318df-0fe9-e911-80cf-9706d383f138</t>
   </si>
   <si>
     <t>^.{0,5}?\.?(\S?\d+(\.\d)?)</t>
+  </si>
+  <si>
+    <t>406d51d6-f83d-ed11-9147-005056b6948b</t>
   </si>
 </sst>
 </file>
@@ -412,7 +397,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,9 +413,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -468,7 +453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -574,7 +559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,24 +709,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C59750-CE11-4137-A397-5E625D311B92}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,19 +737,19 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
-        <v>98</v>
-      </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -775,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -786,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -797,7 +782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -808,7 +793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -819,7 +804,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -830,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -841,7 +826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -852,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -863,7 +848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -874,7 +859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -885,7 +870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -896,7 +881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -907,7 +892,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -918,9 +903,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -929,7 +914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -940,73 +925,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>54</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>55</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1017,18 +1002,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1039,7 +1024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1050,7 +1035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1061,95 +1046,95 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>72</v>
       </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
         <v>74</v>
       </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34">
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
         <v>80</v>
       </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1160,7 +1145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1182,7 +1167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1193,7 +1178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1204,99 +1189,99 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
         <v>86</v>
       </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>88</v>
       </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
         <v>92</v>
       </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E47" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48">
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" t="s">
         <v>99</v>
       </c>
-      <c r="E48" t="s">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
       <c r="B49">
         <v>2</v>
       </c>
@@ -1304,33 +1289,10 @@
         <v>3</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50">
-        <v>8</v>
-      </c>
-      <c r="C50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-      <c r="F50" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G50" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>